<commit_message>
added punt as input
created new fields '01_gwsw'
also fixed StapAllemaal
</commit_message>
<xml_diff>
--- a/inp_fields.xlsx
+++ b/inp_fields.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\02_Werkplaatsen\07_IAN\bk\projecten\GeoDynGem\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BE83F9-CD5C-4876-A686-220AADB01139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CCE076-9259-4A4E-AF82-54D4E8DC07A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="90" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inp_fields" sheetId="1" r:id="rId1"/>
     <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inp_fields!$A$1:$M$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inp_fields!$A$1:$M$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="314">
   <si>
     <t>order</t>
   </si>
@@ -101,18 +101,6 @@
     <t>POC_O_M3_O</t>
   </si>
   <si>
-    <t>AW_15_24_G</t>
-  </si>
-  <si>
-    <t>AW_15_24_O</t>
-  </si>
-  <si>
-    <t>AW_25_50_G</t>
-  </si>
-  <si>
-    <t>AW_25_50_O</t>
-  </si>
-  <si>
     <t>HA_GEM_G</t>
   </si>
   <si>
@@ -233,9 +221,6 @@
     <t>DOUBLE</t>
   </si>
   <si>
-    <t>Geïnstalleerde capaciteit Rg (m3/h)</t>
-  </si>
-  <si>
     <t>Geïnstalleerde capaciteit uit Kikker</t>
   </si>
   <si>
@@ -275,9 +260,6 @@
     <t>POC beschikbaar (T) (m3/h)</t>
   </si>
   <si>
-    <t>[K_INST_TOT] - [DWR_GEBIED] - [IN_DWA_POC]</t>
-  </si>
-  <si>
     <t>Beschikbare Pomp Over Capaciteit (Totaal) in m3/h</t>
   </si>
   <si>
@@ -314,9 +296,6 @@
     <t>K_BR_ST_M3</t>
   </si>
   <si>
-    <t>Berging stelsel (G) (m3)</t>
-  </si>
-  <si>
     <t>Inhoud stelsel uit Kikker in m3</t>
   </si>
   <si>
@@ -329,9 +308,6 @@
     <t>Berging stelsel (G) (mm)</t>
   </si>
   <si>
-    <t>[K_BR_ST_M3]/[HA_TOT_G]/10</t>
-  </si>
-  <si>
     <t>Inhoud stelsel uit Kikker in berekend in mm</t>
   </si>
   <si>
@@ -341,9 +317,6 @@
     <t>Vultijd (uur, (tijdens droogweer))</t>
   </si>
   <si>
-    <t>[K_BR_ST_M3]/[DWR_TOT]</t>
-  </si>
-  <si>
     <t>Inhoud gedeeld door aanvoer (Berging / DWA) in uur</t>
   </si>
   <si>
@@ -356,9 +329,6 @@
     <t>Ledigingstijd (uur) na bui</t>
   </si>
   <si>
-    <t xml:space="preserve"> if([K_BR_ST_M3]/[POC_B_M3_T]&lt; 10,  [K_BR_ST_M3]/[POC_B_M3_T], 10 + ([K_BR_ST_M3] - 10*[POC_B_M3_T])/ [K_INST_TOT])</t>
-  </si>
-  <si>
     <t>Ledigingstijd is de tijd die nodig is om het stelsel te ledigen. Hierbij gaan we ervanuit dat stelsel 10uur lang de DWA en de POC uit de onderbemalingen krijgt. Na 10 uur is er geen DWA en POC meer uit onderbemalingen omdat er niet meer dan 10uur DWA in een dag zit en we er vanuit mogen gaan dat de onderbemaling geen POC meer heeft omdat deze leeg zijn.</t>
   </si>
   <si>
@@ -476,27 +446,9 @@
     <t>DWA berekend op basis van aantal ve's Totaal</t>
   </si>
   <si>
-    <t>AW_15_24_T</t>
-  </si>
-  <si>
-    <t>X Afvw. t/m 2024 (T) (m3/u)</t>
-  </si>
-  <si>
-    <t>[AW_15_24_G]+[AW_15_24_O]</t>
-  </si>
-  <si>
     <t>Extra afvalwater uitbreidingsgebieden Totaal, t/m 2024</t>
   </si>
   <si>
-    <t>AW_25_50_T</t>
-  </si>
-  <si>
-    <t>X Afvw. 25 t/m 50 (T) (m3/u)</t>
-  </si>
-  <si>
-    <t>[AW_25_50_G]+[AW_25_50_O]</t>
-  </si>
-  <si>
     <t>Extra afvalwater uitbreidingsgebieden Totaal, van 2025 t/m 2050</t>
   </si>
   <si>
@@ -587,30 +539,9 @@
     <t>Som ontwerp POC uit onderbemaling</t>
   </si>
   <si>
-    <t>X Afvw. t/m 2024 (G) (m3/u)</t>
-  </si>
-  <si>
-    <t>Extra afvalwater uitbreidingsgebieden uit Gebied, t/m 2024</t>
-  </si>
-  <si>
-    <t>X Afvw. t/m 2024 (O) (m3/u)</t>
-  </si>
-  <si>
-    <t>Extra afvalwater uitbreidingsgebieden uit Onderbemalingen, t/m 2024</t>
-  </si>
-  <si>
-    <t>X Afvw. 25 t/m 50 (G) (m3/u)</t>
-  </si>
-  <si>
     <t>Extra afvalwater uitbreidingsgebieden uit Gebied, van 2025 t/m 2050</t>
   </si>
   <si>
-    <t>X Afvw. 25 t/m 50 (O) (m3/u)</t>
-  </si>
-  <si>
-    <t>Extra afvalwater uitbreidingsgebieden uit Onderbemalingen, van 2025 t/m 2050</t>
-  </si>
-  <si>
     <t>Uit layer vlakkenkaart, van attribuut 'AANSLUIT' neem 'gemengd' en bereken daar het totaal van en deel dat door 10000.</t>
   </si>
   <si>
@@ -785,12 +716,6 @@
     <t>X Afvw. 40 t/m 50 (G) (m3/u)</t>
   </si>
   <si>
-    <t>[Extra_AFW__sum]</t>
-  </si>
-  <si>
-    <t>[Extra_AFW1_sum]</t>
-  </si>
-  <si>
     <t>[ExAFW_2124_sum]</t>
   </si>
   <si>
@@ -942,6 +867,117 @@
   </si>
   <si>
     <t>Totaal aan verhard oppervlak aangesloten op onbekend in gebied (ha)</t>
+  </si>
+  <si>
+    <t>AW_21_24_T</t>
+  </si>
+  <si>
+    <t>AW_25_29_T</t>
+  </si>
+  <si>
+    <t>AW_30_39_T</t>
+  </si>
+  <si>
+    <t>AW_40_50_T</t>
+  </si>
+  <si>
+    <t>X Afvw. 21 t/m 24 (T) (m3/u)</t>
+  </si>
+  <si>
+    <t>X Afvw. 25 t/m 29 (T) (m3/u)</t>
+  </si>
+  <si>
+    <t>X Afvw. 30 t/m 39 (T) (m3/u)</t>
+  </si>
+  <si>
+    <t>X Afvw. 40 t/m 50 (T) (m3/u)</t>
+  </si>
+  <si>
+    <t>[AW_21_24_G]+[AW_21_24_O]</t>
+  </si>
+  <si>
+    <t>[AW_25_29_G]+[AW_25_29_O]</t>
+  </si>
+  <si>
+    <t>[AW_30_39_G]+[AW_30_39_O]</t>
+  </si>
+  <si>
+    <t>[AW_40_50_G]+[AW_40_50_O]</t>
+  </si>
+  <si>
+    <t>TTOTAAL_M3</t>
+  </si>
+  <si>
+    <t>BergendVermogen</t>
+  </si>
+  <si>
+    <t>Berging stelsel Kikker (G) (m3)</t>
+  </si>
+  <si>
+    <t>Berging stelsel berekend (G) (m3)</t>
+  </si>
+  <si>
+    <t>01_gwsw</t>
+  </si>
+  <si>
+    <t>GWSW</t>
+  </si>
+  <si>
+    <t>AantalPompen</t>
+  </si>
+  <si>
+    <t>AantalOverstorten</t>
+  </si>
+  <si>
+    <t>AantalDoorlaaten</t>
+  </si>
+  <si>
+    <t>POMPEN_ST</t>
+  </si>
+  <si>
+    <t>OVERSTORT_</t>
+  </si>
+  <si>
+    <t>DOORLAAT_S</t>
+  </si>
+  <si>
+    <t>MinOverstortdrempel</t>
+  </si>
+  <si>
+    <t>AantalStrengen</t>
+  </si>
+  <si>
+    <t>AantalKnopen</t>
+  </si>
+  <si>
+    <t>Pompcapaciteit_m3_d</t>
+  </si>
+  <si>
+    <t>STRENGEN_S</t>
+  </si>
+  <si>
+    <t>KNOPEN_ST</t>
+  </si>
+  <si>
+    <t>pompcapaciteit * 3,6</t>
+  </si>
+  <si>
+    <t>Pompcapaciteit (m3/dag)</t>
+  </si>
+  <si>
+    <t>[Pompcapaciteit_m3_d] - [DWR_GEBIED] - [IN_DWA_POC]</t>
+  </si>
+  <si>
+    <t>Geïnstalleerde capaciteit Rg kikker (m3/h)</t>
+  </si>
+  <si>
+    <t>[BergendVermogen]/[HA_TOT_G]/10</t>
+  </si>
+  <si>
+    <t>[BergendVermogen]/[DWR_TOT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if([BergendVermogen]/[POC_B_M3_T]&lt; 10,  [BergendVermogen]/[POC_B_M3_T], 10 + ([BergendVermogen] - 10*[POC_B_M3_T])/ [Pompcapaciteit_m3_d])</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1103,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1247,12 +1283,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1414,9 +1444,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1772,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A2" sqref="A2:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -1832,25 +1861,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" t="s">
-        <v>57</v>
-      </c>
       <c r="M2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
@@ -1858,25 +1887,25 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
@@ -1884,25 +1913,25 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="K4" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
@@ -1910,28 +1939,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>1000</v>
       </c>
       <c r="H5" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
@@ -1939,28 +1968,28 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G6">
         <v>1000</v>
       </c>
       <c r="H6" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -1968,31 +1997,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="K7" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="M7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
@@ -2000,28 +2029,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G8">
         <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="M8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
@@ -2032,25 +2061,25 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="I9" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="K9" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="M9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
@@ -2061,83 +2090,83 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E10" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="I10" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="K10" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="M10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
+      <c r="C11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" t="s">
+        <v>226</v>
+      </c>
+      <c r="K11" t="s">
+        <v>167</v>
+      </c>
+      <c r="M11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>58</v>
+      <c r="C12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I12" t="s">
+        <v>227</v>
+      </c>
+      <c r="K12" t="s">
+        <v>167</v>
+      </c>
+      <c r="M12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
@@ -2145,28 +2174,28 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H13" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="I13" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="K13" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
@@ -2174,28 +2203,28 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="I14" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="K14" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
@@ -2203,28 +2232,28 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="I15" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="K15" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="M15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
@@ -2232,28 +2261,28 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="I16" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="K16" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
@@ -2261,86 +2290,89 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="I17" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="K17" t="s">
-        <v>235</v>
+        <v>150</v>
       </c>
       <c r="M17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
       <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E18" t="s">
-        <v>239</v>
-      </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>236</v>
-      </c>
-      <c r="I18" t="s">
-        <v>238</v>
+        <v>46</v>
       </c>
       <c r="K18" t="s">
-        <v>237</v>
+        <v>47</v>
       </c>
       <c r="M18" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>165</v>
-      </c>
-      <c r="I19" t="s">
-        <v>257</v>
+        <v>310</v>
       </c>
       <c r="K19" t="s">
-        <v>166</v>
+        <v>61</v>
       </c>
       <c r="M19" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
@@ -2348,31 +2380,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" t="s">
         <v>48</v>
-      </c>
-      <c r="F20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20">
-        <v>50</v>
-      </c>
-      <c r="H20" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" t="s">
-        <v>51</v>
-      </c>
-      <c r="M20" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.15">
@@ -2380,28 +2409,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" t="s">
+        <v>291</v>
+      </c>
+      <c r="K21" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21" t="s">
         <v>48</v>
-      </c>
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" t="s">
-        <v>66</v>
-      </c>
-      <c r="M21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
@@ -2409,28 +2438,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>197</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="M22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
@@ -2438,28 +2467,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>197</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" t="s">
+        <v>200</v>
+      </c>
+      <c r="K23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M23" t="s">
         <v>48</v>
-      </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" t="s">
-        <v>92</v>
-      </c>
-      <c r="K23" t="s">
-        <v>93</v>
-      </c>
-      <c r="M23" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
@@ -2467,28 +2496,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>206</v>
+      </c>
+      <c r="K24" t="s">
+        <v>206</v>
+      </c>
+      <c r="M24" t="s">
         <v>48</v>
-      </c>
-      <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" t="s">
-        <v>221</v>
-      </c>
-      <c r="K24" t="s">
-        <v>222</v>
-      </c>
-      <c r="M24" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.15">
@@ -2496,60 +2528,63 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>220</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>290</v>
       </c>
       <c r="D25" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>293</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
-        <v>223</v>
+        <v>292</v>
+      </c>
+      <c r="I25" t="s">
+        <v>84</v>
       </c>
       <c r="K25" t="s">
-        <v>224</v>
+        <v>292</v>
       </c>
       <c r="M25" t="s">
-        <v>52</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>228</v>
-      </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>304</v>
       </c>
       <c r="D26" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>293</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H26" t="s">
-        <v>229</v>
+        <v>308</v>
+      </c>
+      <c r="I26" t="s">
+        <v>58</v>
       </c>
       <c r="K26" t="s">
-        <v>229</v>
+        <v>304</v>
+      </c>
+      <c r="L26" t="s">
+        <v>307</v>
       </c>
       <c r="M26" t="s">
-        <v>52</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.15">
@@ -2557,28 +2592,28 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>301</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H27" t="s">
-        <v>168</v>
+        <v>301</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="K27" t="s">
-        <v>169</v>
+        <v>301</v>
       </c>
       <c r="M27" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.15">
@@ -2586,28 +2621,28 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>295</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H28" t="s">
-        <v>172</v>
+        <v>295</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>298</v>
       </c>
       <c r="K28" t="s">
-        <v>173</v>
+        <v>295</v>
       </c>
       <c r="M28" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.15">
@@ -2615,28 +2650,28 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>296</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H29" t="s">
-        <v>176</v>
+        <v>296</v>
       </c>
       <c r="I29" t="s">
-        <v>17</v>
+        <v>299</v>
       </c>
       <c r="K29" t="s">
-        <v>177</v>
+        <v>296</v>
       </c>
       <c r="M29" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
@@ -2644,28 +2679,28 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>297</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>185</v>
+        <v>297</v>
       </c>
       <c r="I30" t="s">
-        <v>21</v>
+        <v>300</v>
       </c>
       <c r="K30" t="s">
-        <v>186</v>
+        <v>297</v>
       </c>
       <c r="M30" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.15">
@@ -2673,28 +2708,28 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>302</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
-        <v>189</v>
+        <v>302</v>
       </c>
       <c r="I31" t="s">
-        <v>23</v>
+        <v>305</v>
       </c>
       <c r="K31" t="s">
-        <v>190</v>
+        <v>302</v>
       </c>
       <c r="M31" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.15">
@@ -2702,28 +2737,28 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="D32" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>245</v>
+        <v>303</v>
       </c>
       <c r="I32" t="s">
-        <v>241</v>
+        <v>306</v>
       </c>
       <c r="K32" t="s">
-        <v>188</v>
+        <v>303</v>
       </c>
       <c r="M32" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
@@ -2731,28 +2766,28 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>259</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E33" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H33" t="s">
-        <v>246</v>
+        <v>152</v>
       </c>
       <c r="I33" t="s">
-        <v>242</v>
+        <v>13</v>
       </c>
       <c r="K33" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="M33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.15">
@@ -2760,28 +2795,28 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>260</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="F34" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H34" t="s">
-        <v>247</v>
+        <v>156</v>
       </c>
       <c r="I34" t="s">
-        <v>243</v>
+        <v>15</v>
       </c>
       <c r="K34" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="M34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.15">
@@ -2789,28 +2824,28 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>261</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E35" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="F35" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s">
-        <v>248</v>
+        <v>160</v>
       </c>
       <c r="I35" t="s">
-        <v>244</v>
+        <v>17</v>
       </c>
       <c r="K35" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="M35" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.15">
@@ -2818,28 +2853,28 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F36" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H36" t="s">
-        <v>73</v>
+        <v>222</v>
       </c>
       <c r="I36" t="s">
-        <v>74</v>
+        <v>218</v>
       </c>
       <c r="K36" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="M36" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
@@ -2847,28 +2882,28 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="D37" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H37" t="s">
-        <v>129</v>
+        <v>223</v>
       </c>
       <c r="I37" t="s">
-        <v>130</v>
+        <v>219</v>
       </c>
       <c r="K37" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="M37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.15">
@@ -2876,28 +2911,28 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>137</v>
+        <v>235</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H38" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="I38" t="s">
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="K38" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="M38" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.15">
@@ -2905,28 +2940,28 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="F39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H39" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="I39" t="s">
-        <v>148</v>
+        <v>221</v>
       </c>
       <c r="K39" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="M39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.15">
@@ -2934,28 +2969,28 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H40" t="s">
-        <v>151</v>
+        <v>68</v>
       </c>
       <c r="I40" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="K40" t="s">
-        <v>153</v>
+        <v>70</v>
       </c>
       <c r="M40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
@@ -2963,28 +2998,28 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E41" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="F41" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="I41" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="K41" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="M41" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
@@ -2992,60 +3027,57 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E42" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="F42" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H42" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I42" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K42" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="M42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>191</v>
-      </c>
       <c r="C43" t="s">
-        <v>25</v>
+        <v>277</v>
       </c>
       <c r="D43" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E43" t="s">
-        <v>280</v>
+        <v>67</v>
       </c>
       <c r="F43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H43" t="s">
-        <v>192</v>
+        <v>281</v>
       </c>
       <c r="I43" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="K43" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="M43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.15">
@@ -3053,92 +3085,86 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>278</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>280</v>
+        <v>67</v>
       </c>
       <c r="F44" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H44" t="s">
-        <v>197</v>
+        <v>282</v>
       </c>
       <c r="I44" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="K44" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="M44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>194</v>
-      </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>279</v>
       </c>
       <c r="D45" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>280</v>
+        <v>67</v>
       </c>
       <c r="F45" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H45" t="s">
-        <v>195</v>
+        <v>283</v>
       </c>
       <c r="I45" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="K45" t="s">
-        <v>196</v>
+        <v>136</v>
       </c>
       <c r="M45" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>191</v>
-      </c>
       <c r="C46" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E46" t="s">
-        <v>280</v>
+        <v>67</v>
       </c>
       <c r="F46" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H46" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I46" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="K46" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="M46" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.15">
@@ -3146,28 +3172,28 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>273</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>280</v>
+        <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H47" t="s">
-        <v>281</v>
+        <v>133</v>
       </c>
       <c r="I47" t="s">
-        <v>274</v>
+        <v>134</v>
       </c>
       <c r="K47" t="s">
-        <v>298</v>
+        <v>135</v>
       </c>
       <c r="M47" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.15">
@@ -3175,57 +3201,60 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>280</v>
+        <v>123</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H48" t="s">
-        <v>282</v>
+        <v>124</v>
       </c>
       <c r="I48" t="s">
-        <v>271</v>
+        <v>125</v>
       </c>
       <c r="K48" t="s">
-        <v>299</v>
+        <v>126</v>
       </c>
       <c r="M48" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" t="s">
+        <v>168</v>
+      </c>
       <c r="C49" t="s">
-        <v>276</v>
+        <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E49" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="F49" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H49" t="s">
-        <v>277</v>
+        <v>169</v>
       </c>
       <c r="I49" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="K49" t="s">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="M49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.15">
@@ -3233,83 +3262,92 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E50" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="F50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H50" t="s">
-        <v>283</v>
+        <v>174</v>
+      </c>
+      <c r="I50" t="s">
+        <v>245</v>
       </c>
       <c r="K50" t="s">
-        <v>301</v>
+        <v>175</v>
       </c>
       <c r="M50" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>50</v>
       </c>
+      <c r="B51" t="s">
+        <v>171</v>
+      </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E51" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="F51" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H51" t="s">
-        <v>284</v>
+        <v>172</v>
       </c>
       <c r="I51" t="s">
-        <v>297</v>
+        <v>244</v>
       </c>
       <c r="K51" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="M51" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>51</v>
       </c>
+      <c r="B52" t="s">
+        <v>168</v>
+      </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>247</v>
       </c>
       <c r="D52" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E52" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="F52" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H52" t="s">
-        <v>200</v>
+        <v>264</v>
       </c>
       <c r="I52" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="K52" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="M52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.15">
@@ -3317,28 +3355,28 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>248</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E53" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="F53" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H53" t="s">
-        <v>109</v>
+        <v>256</v>
       </c>
       <c r="I53" t="s">
-        <v>110</v>
+        <v>249</v>
       </c>
       <c r="K53" t="s">
-        <v>111</v>
+        <v>273</v>
       </c>
       <c r="M53" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.15">
@@ -3346,31 +3384,28 @@
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E54" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="F54" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H54" t="s">
-        <v>202</v>
+        <v>257</v>
       </c>
       <c r="I54" t="s">
-        <v>203</v>
-      </c>
-      <c r="J54" t="s">
-        <v>30</v>
+        <v>246</v>
       </c>
       <c r="K54" t="s">
-        <v>204</v>
+        <v>274</v>
       </c>
       <c r="M54" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.15">
@@ -3378,31 +3413,28 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>251</v>
       </c>
       <c r="D55" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E55" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="F55" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H55" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
       <c r="I55" t="s">
-        <v>206</v>
-      </c>
-      <c r="J55" t="s">
-        <v>30</v>
+        <v>253</v>
       </c>
       <c r="K55" t="s">
-        <v>207</v>
+        <v>275</v>
       </c>
       <c r="M55" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.15">
@@ -3410,31 +3442,25 @@
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E56" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="F56" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H56" t="s">
-        <v>208</v>
-      </c>
-      <c r="I56" t="s">
-        <v>209</v>
-      </c>
-      <c r="J56" t="s">
-        <v>30</v>
+        <v>258</v>
       </c>
       <c r="K56" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="M56" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.15">
@@ -3442,31 +3468,28 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="F57" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H57" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="I57" t="s">
-        <v>212</v>
-      </c>
-      <c r="J57" t="s">
-        <v>30</v>
+        <v>272</v>
       </c>
       <c r="K57" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="M57" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.15">
@@ -3474,31 +3497,28 @@
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>290</v>
+        <v>27</v>
       </c>
       <c r="D58" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E58" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="F58" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H58" t="s">
-        <v>293</v>
+        <v>177</v>
       </c>
       <c r="I58" t="s">
-        <v>294</v>
-      </c>
-      <c r="J58" t="s">
-        <v>30</v>
+        <v>254</v>
       </c>
       <c r="K58" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="M58" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.15">
@@ -3506,31 +3526,28 @@
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>291</v>
+        <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E59" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F59" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H59" t="s">
-        <v>292</v>
+        <v>99</v>
       </c>
       <c r="I59" t="s">
-        <v>295</v>
-      </c>
-      <c r="J59" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="K59" t="s">
-        <v>215</v>
+        <v>101</v>
       </c>
       <c r="M59" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.15">
@@ -3538,31 +3555,31 @@
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E60" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F60" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H60" t="s">
-        <v>285</v>
+        <v>179</v>
       </c>
       <c r="I60" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="J60" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K60" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="M60" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.15">
@@ -3570,31 +3587,31 @@
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>286</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E61" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F61" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H61" t="s">
-        <v>287</v>
+        <v>182</v>
       </c>
       <c r="I61" t="s">
-        <v>288</v>
+        <v>183</v>
       </c>
       <c r="J61" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K61" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="M61" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.15">
@@ -3602,31 +3619,31 @@
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E62" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F62" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H62" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="I62" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="J62" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K62" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="M62" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.15">
@@ -3634,31 +3651,31 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F63" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H63" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="I63" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="J63" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="K63" t="s">
-        <v>98</v>
+        <v>190</v>
       </c>
       <c r="M63" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.15">
@@ -3666,31 +3683,31 @@
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>265</v>
       </c>
       <c r="D64" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E64" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F64" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H64" t="s">
-        <v>100</v>
+        <v>268</v>
       </c>
       <c r="I64" t="s">
-        <v>101</v>
+        <v>269</v>
       </c>
       <c r="J64" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="K64" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
       <c r="M64" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.15">
@@ -3698,31 +3715,31 @@
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>112</v>
+        <v>266</v>
       </c>
       <c r="D65" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E65" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F65" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H65" t="s">
-        <v>113</v>
+        <v>267</v>
       </c>
       <c r="I65" t="s">
-        <v>114</v>
+        <v>270</v>
       </c>
       <c r="J65" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="K65" t="s">
-        <v>115</v>
+        <v>192</v>
       </c>
       <c r="M65" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.15">
@@ -3730,28 +3747,31 @@
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D66" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E66" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F66" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H66" t="s">
-        <v>178</v>
+        <v>260</v>
       </c>
       <c r="I66" t="s">
-        <v>179</v>
+        <v>191</v>
+      </c>
+      <c r="J66" t="s">
+        <v>26</v>
       </c>
       <c r="K66" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="M66" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.15">
@@ -3759,31 +3779,31 @@
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="D67" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E67" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F67" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H67" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="I67" t="s">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="J67" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="K67" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="M67" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.15">
@@ -3791,28 +3811,31 @@
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D68" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E68" t="s">
-        <v>267</v>
+        <v>98</v>
       </c>
       <c r="F68" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H68" t="s">
-        <v>69</v>
+        <v>194</v>
       </c>
       <c r="I68" t="s">
-        <v>63</v>
+        <v>195</v>
+      </c>
+      <c r="J68" t="s">
+        <v>26</v>
       </c>
       <c r="K68" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="M68" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.15">
@@ -3820,28 +3843,31 @@
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="D69" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E69" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="F69" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H69" t="s">
-        <v>181</v>
+        <v>89</v>
       </c>
       <c r="I69" t="s">
-        <v>19</v>
+        <v>311</v>
+      </c>
+      <c r="J69" t="s">
+        <v>78</v>
       </c>
       <c r="K69" t="s">
-        <v>182</v>
+        <v>90</v>
       </c>
       <c r="M69" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.15">
@@ -3849,28 +3875,31 @@
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D70" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E70" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F70" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H70" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="I70" t="s">
-        <v>79</v>
+        <v>312</v>
+      </c>
+      <c r="J70" t="s">
+        <v>66</v>
       </c>
       <c r="K70" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="M70" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.15">
@@ -3878,31 +3907,31 @@
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D71" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E71" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F71" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H71" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="I71" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="J71" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="K71" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="M71" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.15">
@@ -3910,28 +3939,28 @@
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
       <c r="D72" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E72" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F72" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H72" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="I72" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="K72" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="M72" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.15">
@@ -3939,28 +3968,31 @@
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="D73" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="F73" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H73" t="s">
-        <v>105</v>
+        <v>202</v>
       </c>
       <c r="I73" t="s">
-        <v>106</v>
+        <v>203</v>
+      </c>
+      <c r="J73" t="s">
+        <v>78</v>
       </c>
       <c r="K73" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="M73" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.15">
@@ -3968,31 +4000,28 @@
         <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="D74" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>242</v>
       </c>
       <c r="F74" t="s">
+        <v>60</v>
+      </c>
+      <c r="H74" t="s">
         <v>64</v>
       </c>
-      <c r="H74" t="s">
-        <v>121</v>
-      </c>
       <c r="I74" t="s">
-        <v>122</v>
-      </c>
-      <c r="J74" t="s">
-        <v>84</v>
+        <v>304</v>
       </c>
       <c r="K74" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="M74" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.15">
@@ -4000,66 +4029,246 @@
         <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E75" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="F75" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H75" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="I75" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="K75" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="M75" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
-        <v>230</v>
-      </c>
       <c r="C76" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D76" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E76" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="F76" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H76" t="s">
-        <v>231</v>
+        <v>73</v>
       </c>
       <c r="I76" t="s">
-        <v>232</v>
+        <v>309</v>
       </c>
       <c r="K76" t="s">
-        <v>233</v>
+        <v>74</v>
       </c>
       <c r="M76" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="C77" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E77" t="s">
+        <v>72</v>
+      </c>
+      <c r="F77" t="s">
+        <v>60</v>
+      </c>
+      <c r="H77" t="s">
+        <v>76</v>
+      </c>
+      <c r="I77" t="s">
+        <v>77</v>
+      </c>
+      <c r="J77" t="s">
+        <v>78</v>
+      </c>
+      <c r="K77" t="s">
+        <v>79</v>
+      </c>
+      <c r="M77" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="C78" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" t="s">
+        <v>43</v>
+      </c>
+      <c r="E78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F78" t="s">
+        <v>60</v>
+      </c>
+      <c r="H78" t="s">
+        <v>107</v>
+      </c>
+      <c r="I78" t="s">
+        <v>108</v>
+      </c>
+      <c r="K78" t="s">
+        <v>109</v>
+      </c>
+      <c r="M78" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" t="s">
+        <v>43</v>
+      </c>
+      <c r="E79" t="s">
+        <v>95</v>
+      </c>
+      <c r="F79" t="s">
+        <v>60</v>
+      </c>
+      <c r="H79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I79" t="s">
+        <v>313</v>
+      </c>
+      <c r="K79" t="s">
+        <v>97</v>
+      </c>
+      <c r="M79" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="C80" t="s">
+        <v>110</v>
+      </c>
+      <c r="D80" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" t="s">
+        <v>60</v>
+      </c>
+      <c r="H80" t="s">
+        <v>111</v>
+      </c>
+      <c r="I80" t="s">
+        <v>112</v>
+      </c>
+      <c r="J80" t="s">
+        <v>78</v>
+      </c>
+      <c r="K80" t="s">
+        <v>113</v>
+      </c>
+      <c r="M80" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="C81" t="s">
+        <v>114</v>
+      </c>
+      <c r="D81" t="s">
+        <v>43</v>
+      </c>
+      <c r="E81" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" t="s">
+        <v>60</v>
+      </c>
+      <c r="H81" t="s">
+        <v>115</v>
+      </c>
+      <c r="I81" t="s">
+        <v>116</v>
+      </c>
+      <c r="K81" t="s">
+        <v>117</v>
+      </c>
+      <c r="M81" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>207</v>
+      </c>
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" t="s">
+        <v>148</v>
+      </c>
+      <c r="E82" t="s">
+        <v>95</v>
+      </c>
+      <c r="F82" t="s">
+        <v>51</v>
+      </c>
+      <c r="H82" t="s">
+        <v>208</v>
+      </c>
+      <c r="I82" t="s">
+        <v>209</v>
+      </c>
+      <c r="K82" t="s">
+        <v>210</v>
+      </c>
+      <c r="M82" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M80" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M80">
-      <sortCondition ref="A1:A80"/>
+  <autoFilter ref="A1:M86" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M86">
+      <sortCondition ref="A1:A86"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4078,12 +4287,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" t="str">
         <f>A1&amp;";"&amp;A2</f>
@@ -4092,7 +4301,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3" t="str">
         <f>B2&amp;";"&amp;A3</f>
@@ -4101,7 +4310,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B10" si="0">B3&amp;";"&amp;A4</f>
@@ -4110,7 +4319,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -4119,7 +4328,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -4128,7 +4337,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -4137,7 +4346,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -4146,7 +4355,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -4155,7 +4364,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -4164,7 +4373,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
always add result on top
and add descriptions to ONTVANGT_VAN
</commit_message>
<xml_diff>
--- a/inp_fields.xlsx
+++ b/inp_fields.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\02_Werkplaatsen\07_IAN\bk\projecten\GeoDynGem\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b_kro\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\GeoDynGemGWSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CCE076-9259-4A4E-AF82-54D4E8DC07A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F025760B-13E2-48D1-BE83-8BA3A37D1214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="90" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inp_fields" sheetId="1" r:id="rId1"/>
     <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inp_fields!$A$1:$M$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inp_fields!$A$1:$M$90</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="322">
   <si>
     <t>order</t>
   </si>
@@ -978,6 +978,30 @@
   </si>
   <si>
     <t xml:space="preserve"> if([BergendVermogen]/[POC_B_M3_T]&lt; 10,  [BergendVermogen]/[POC_B_M3_T], 10 + ([BergendVermogen] - 10*[POC_B_M3_T])/ [Pompcapaciteit_m3_d])</t>
+  </si>
+  <si>
+    <t>K_ONTV_VAN_NAME</t>
+  </si>
+  <si>
+    <t>K_ONTV_1N_NAME</t>
+  </si>
+  <si>
+    <t>K_LOOST_OP_NAME</t>
+  </si>
+  <si>
+    <t>K_KNP_EIND_NAME</t>
+  </si>
+  <si>
+    <t>Ontvangt van bemid</t>
+  </si>
+  <si>
+    <t>Ontvangt direct van bemid</t>
+  </si>
+  <si>
+    <t>Loost op bemid</t>
+  </si>
+  <si>
+    <t>Eindbemalingsgebied bemid</t>
   </si>
 </sst>
 </file>
@@ -1801,21 +1825,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A82"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" customWidth="1"/>
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.75" customWidth="1"/>
+    <col min="9" max="9" width="33.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1856,7 +1881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1882,7 +1907,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1908,7 +1933,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1934,7 +1959,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1954,7 +1979,7 @@
         <v>1000</v>
       </c>
       <c r="H5" t="s">
-        <v>139</v>
+        <v>318</v>
       </c>
       <c r="K5" t="s">
         <v>140</v>
@@ -1963,7 +1988,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1983,7 +2008,7 @@
         <v>1000</v>
       </c>
       <c r="H6" t="s">
-        <v>238</v>
+        <v>319</v>
       </c>
       <c r="K6" t="s">
         <v>140</v>
@@ -1992,7 +2017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2015,7 +2040,7 @@
         <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>320</v>
       </c>
       <c r="K7" t="s">
         <v>144</v>
@@ -2024,7 +2049,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2044,7 +2069,7 @@
         <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>146</v>
+        <v>321</v>
       </c>
       <c r="K8" t="s">
         <v>147</v>
@@ -2053,128 +2078,131 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>1000</v>
       </c>
       <c r="H9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I9" t="s">
-        <v>230</v>
+        <v>139</v>
       </c>
       <c r="K9" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="M9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>315</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>1000</v>
       </c>
       <c r="H10" t="s">
-        <v>158</v>
-      </c>
-      <c r="I10" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="K10" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="M10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>141</v>
+      </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>316</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>216</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>222</v>
-      </c>
-      <c r="I11" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
       <c r="K11" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="M11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>317</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>216</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12">
         <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>223</v>
-      </c>
-      <c r="I12" t="s">
-        <v>227</v>
+        <v>146</v>
       </c>
       <c r="K12" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>148</v>
@@ -2183,27 +2211,27 @@
         <v>216</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
-        <v>224</v>
+        <v>154</v>
       </c>
       <c r="I13" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="K13" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="M13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>148</v>
@@ -2212,27 +2240,27 @@
         <v>216</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H14" t="s">
-        <v>225</v>
+        <v>158</v>
       </c>
       <c r="I14" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="K14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="M14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="D15" t="s">
         <v>148</v>
@@ -2244,24 +2272,24 @@
         <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="I15" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="K15" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="M15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>219</v>
       </c>
       <c r="D16" t="s">
         <v>148</v>
@@ -2273,24 +2301,24 @@
         <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="I16" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="K16" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="M16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>220</v>
       </c>
       <c r="D17" t="s">
         <v>148</v>
@@ -2302,178 +2330,178 @@
         <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>149</v>
+        <v>224</v>
       </c>
       <c r="I17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K17" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="M17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>221</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>225</v>
+      </c>
+      <c r="I18" t="s">
+        <v>229</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="M18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="F19" t="s">
         <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>310</v>
+        <v>211</v>
+      </c>
+      <c r="I19" t="s">
+        <v>217</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>212</v>
       </c>
       <c r="M19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>80</v>
-      </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>213</v>
+      </c>
+      <c r="I20" t="s">
+        <v>215</v>
       </c>
       <c r="K20" t="s">
-        <v>83</v>
+        <v>214</v>
       </c>
       <c r="M20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>84</v>
-      </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="F21" t="s">
         <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>291</v>
+        <v>149</v>
+      </c>
+      <c r="I21" t="s">
+        <v>232</v>
       </c>
       <c r="K21" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="M21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="G22">
+        <v>50</v>
       </c>
       <c r="H22" t="s">
-        <v>198</v>
+        <v>46</v>
       </c>
       <c r="K22" t="s">
-        <v>199</v>
+        <v>47</v>
       </c>
       <c r="M22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
         <v>44</v>
@@ -2482,175 +2510,172 @@
         <v>60</v>
       </c>
       <c r="H23" t="s">
-        <v>200</v>
+        <v>310</v>
       </c>
       <c r="K23" t="s">
-        <v>201</v>
+        <v>61</v>
       </c>
       <c r="M23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H24" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="K24" t="s">
-        <v>206</v>
+        <v>83</v>
       </c>
       <c r="M24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>289</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>290</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
         <v>60</v>
       </c>
       <c r="H25" t="s">
-        <v>292</v>
-      </c>
-      <c r="I25" t="s">
-        <v>84</v>
+        <v>291</v>
       </c>
       <c r="K25" t="s">
-        <v>292</v>
+        <v>86</v>
       </c>
       <c r="M25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>197</v>
+      </c>
       <c r="C26" t="s">
-        <v>304</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E26" t="s">
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
         <v>60</v>
       </c>
       <c r="H26" t="s">
-        <v>308</v>
-      </c>
-      <c r="I26" t="s">
-        <v>58</v>
+        <v>198</v>
       </c>
       <c r="K26" t="s">
-        <v>304</v>
-      </c>
-      <c r="L26" t="s">
-        <v>307</v>
+        <v>199</v>
       </c>
       <c r="M26" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>197</v>
+      </c>
       <c r="C27" t="s">
-        <v>301</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
         <v>60</v>
       </c>
       <c r="H27" t="s">
-        <v>301</v>
-      </c>
-      <c r="I27" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="K27" t="s">
-        <v>301</v>
+        <v>201</v>
       </c>
       <c r="M27" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
       <c r="C28" t="s">
-        <v>295</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E28" t="s">
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
       </c>
       <c r="H28" t="s">
-        <v>295</v>
-      </c>
-      <c r="I28" t="s">
-        <v>298</v>
+        <v>206</v>
       </c>
       <c r="K28" t="s">
-        <v>295</v>
+        <v>206</v>
       </c>
       <c r="M28" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>289</v>
+      </c>
       <c r="C29" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D29" t="s">
         <v>43</v>
@@ -2659,27 +2684,27 @@
         <v>293</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I29" t="s">
-        <v>299</v>
+        <v>84</v>
       </c>
       <c r="K29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="M29" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D30" t="s">
         <v>43</v>
@@ -2688,27 +2713,30 @@
         <v>293</v>
       </c>
       <c r="F30" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H30" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="I30" t="s">
-        <v>300</v>
+        <v>58</v>
       </c>
       <c r="K30" t="s">
-        <v>297</v>
+        <v>304</v>
+      </c>
+      <c r="L30" t="s">
+        <v>307</v>
       </c>
       <c r="M30" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D31" t="s">
         <v>43</v>
@@ -2717,27 +2745,27 @@
         <v>293</v>
       </c>
       <c r="F31" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I31" t="s">
-        <v>305</v>
+        <v>80</v>
       </c>
       <c r="K31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M31" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="D32" t="s">
         <v>43</v>
@@ -2749,140 +2777,140 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I32" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="K32" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="M32" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>296</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>151</v>
+        <v>293</v>
       </c>
       <c r="F33" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H33" t="s">
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="I33" t="s">
-        <v>13</v>
+        <v>299</v>
       </c>
       <c r="K33" t="s">
-        <v>153</v>
+        <v>296</v>
       </c>
       <c r="M33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>297</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>151</v>
+        <v>293</v>
       </c>
       <c r="F34" t="s">
         <v>51</v>
       </c>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>297</v>
       </c>
       <c r="I34" t="s">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="K34" t="s">
-        <v>157</v>
+        <v>297</v>
       </c>
       <c r="M34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>302</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>151</v>
+        <v>293</v>
       </c>
       <c r="F35" t="s">
         <v>51</v>
       </c>
       <c r="H35" t="s">
-        <v>160</v>
+        <v>302</v>
       </c>
       <c r="I35" t="s">
-        <v>17</v>
+        <v>305</v>
       </c>
       <c r="K35" t="s">
-        <v>161</v>
+        <v>302</v>
       </c>
       <c r="M35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>233</v>
+        <v>303</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>151</v>
+        <v>293</v>
       </c>
       <c r="F36" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H36" t="s">
-        <v>222</v>
+        <v>303</v>
       </c>
       <c r="I36" t="s">
-        <v>218</v>
+        <v>306</v>
       </c>
       <c r="K36" t="s">
-        <v>167</v>
+        <v>303</v>
       </c>
       <c r="M36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>234</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
         <v>148</v>
@@ -2894,24 +2922,24 @@
         <v>60</v>
       </c>
       <c r="H37" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="I37" t="s">
-        <v>219</v>
+        <v>13</v>
       </c>
       <c r="K37" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="M37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>235</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
         <v>148</v>
@@ -2920,27 +2948,27 @@
         <v>151</v>
       </c>
       <c r="F38" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H38" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="I38" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="K38" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="M38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>236</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
         <v>148</v>
@@ -2949,143 +2977,143 @@
         <v>151</v>
       </c>
       <c r="F39" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H39" t="s">
-        <v>225</v>
+        <v>160</v>
       </c>
       <c r="I39" t="s">
-        <v>221</v>
+        <v>17</v>
       </c>
       <c r="K39" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="M39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>233</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="F40" t="s">
         <v>60</v>
       </c>
       <c r="H40" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
       <c r="I40" t="s">
-        <v>69</v>
+        <v>218</v>
       </c>
       <c r="K40" t="s">
-        <v>70</v>
+        <v>167</v>
       </c>
       <c r="M40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>234</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E41" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="F41" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H41" t="s">
-        <v>119</v>
+        <v>223</v>
       </c>
       <c r="I41" t="s">
-        <v>120</v>
+        <v>219</v>
       </c>
       <c r="K41" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="M41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="F42" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H42" t="s">
-        <v>128</v>
+        <v>224</v>
       </c>
       <c r="I42" t="s">
-        <v>129</v>
+        <v>220</v>
       </c>
       <c r="K42" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="M42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>277</v>
+        <v>236</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E43" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="F43" t="s">
         <v>60</v>
       </c>
       <c r="H43" t="s">
-        <v>281</v>
+        <v>225</v>
       </c>
       <c r="I43" t="s">
-        <v>285</v>
+        <v>221</v>
       </c>
       <c r="K43" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="M43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>278</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
         <v>43</v>
@@ -3097,24 +3125,24 @@
         <v>60</v>
       </c>
       <c r="H44" t="s">
-        <v>282</v>
+        <v>68</v>
       </c>
       <c r="I44" t="s">
-        <v>286</v>
+        <v>69</v>
       </c>
       <c r="K44" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="M44" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>279</v>
+        <v>118</v>
       </c>
       <c r="D45" t="s">
         <v>43</v>
@@ -3123,27 +3151,27 @@
         <v>67</v>
       </c>
       <c r="F45" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H45" t="s">
-        <v>283</v>
+        <v>119</v>
       </c>
       <c r="I45" t="s">
-        <v>287</v>
+        <v>120</v>
       </c>
       <c r="K45" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="M45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>280</v>
+        <v>127</v>
       </c>
       <c r="D46" t="s">
         <v>43</v>
@@ -3152,210 +3180,204 @@
         <v>67</v>
       </c>
       <c r="F46" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H46" t="s">
-        <v>284</v>
+        <v>128</v>
       </c>
       <c r="I46" t="s">
-        <v>288</v>
+        <v>129</v>
       </c>
       <c r="K46" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="M46" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="D47" t="s">
         <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>132</v>
+        <v>67</v>
       </c>
       <c r="F47" t="s">
         <v>60</v>
       </c>
       <c r="H47" t="s">
-        <v>133</v>
+        <v>281</v>
       </c>
       <c r="I47" t="s">
-        <v>134</v>
+        <v>285</v>
       </c>
       <c r="K47" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>278</v>
       </c>
       <c r="D48" t="s">
         <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="F48" t="s">
         <v>60</v>
       </c>
       <c r="H48" t="s">
-        <v>124</v>
+        <v>282</v>
       </c>
       <c r="I48" t="s">
-        <v>125</v>
+        <v>286</v>
       </c>
       <c r="K48" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="M48" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>168</v>
-      </c>
       <c r="C49" t="s">
-        <v>21</v>
+        <v>279</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E49" t="s">
-        <v>255</v>
+        <v>67</v>
       </c>
       <c r="F49" t="s">
         <v>60</v>
       </c>
       <c r="H49" t="s">
-        <v>169</v>
+        <v>283</v>
       </c>
       <c r="I49" t="s">
-        <v>243</v>
+        <v>287</v>
       </c>
       <c r="K49" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="M49" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>280</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E50" t="s">
-        <v>255</v>
+        <v>67</v>
       </c>
       <c r="F50" t="s">
         <v>60</v>
       </c>
       <c r="H50" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
       <c r="I50" t="s">
-        <v>245</v>
+        <v>288</v>
       </c>
       <c r="K50" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="M50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
-        <v>171</v>
-      </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E51" t="s">
-        <v>255</v>
+        <v>132</v>
       </c>
       <c r="F51" t="s">
         <v>60</v>
       </c>
       <c r="H51" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="I51" t="s">
-        <v>244</v>
+        <v>134</v>
       </c>
       <c r="K51" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="M51" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
-        <v>168</v>
-      </c>
       <c r="C52" t="s">
-        <v>247</v>
+        <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E52" t="s">
-        <v>255</v>
+        <v>123</v>
       </c>
       <c r="F52" t="s">
         <v>60</v>
       </c>
       <c r="H52" t="s">
-        <v>264</v>
+        <v>124</v>
       </c>
       <c r="I52" t="s">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="K52" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="M52" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
+      <c r="B53" t="s">
+        <v>168</v>
+      </c>
       <c r="C53" t="s">
-        <v>248</v>
+        <v>21</v>
       </c>
       <c r="D53" t="s">
         <v>148</v>
@@ -3367,24 +3389,24 @@
         <v>60</v>
       </c>
       <c r="H53" t="s">
-        <v>256</v>
+        <v>169</v>
       </c>
       <c r="I53" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="K53" t="s">
-        <v>273</v>
+        <v>170</v>
       </c>
       <c r="M53" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
         <v>148</v>
@@ -3396,24 +3418,27 @@
         <v>60</v>
       </c>
       <c r="H54" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="I54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K54" t="s">
-        <v>274</v>
+        <v>175</v>
       </c>
       <c r="M54" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
+      <c r="B55" t="s">
+        <v>171</v>
+      </c>
       <c r="C55" t="s">
-        <v>251</v>
+        <v>22</v>
       </c>
       <c r="D55" t="s">
         <v>148</v>
@@ -3425,24 +3450,27 @@
         <v>60</v>
       </c>
       <c r="H55" t="s">
-        <v>252</v>
+        <v>172</v>
       </c>
       <c r="I55" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K55" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="M55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56" t="s">
+        <v>168</v>
+      </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>247</v>
       </c>
       <c r="D56" t="s">
         <v>148</v>
@@ -3454,21 +3482,24 @@
         <v>60</v>
       </c>
       <c r="H56" t="s">
-        <v>258</v>
+        <v>264</v>
+      </c>
+      <c r="I56" t="s">
+        <v>250</v>
       </c>
       <c r="K56" t="s">
-        <v>276</v>
+        <v>170</v>
       </c>
       <c r="M56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>248</v>
       </c>
       <c r="D57" t="s">
         <v>148</v>
@@ -3480,24 +3511,24 @@
         <v>60</v>
       </c>
       <c r="H57" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I57" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="K57" t="s">
-        <v>176</v>
+        <v>273</v>
       </c>
       <c r="M57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D58" t="s">
         <v>148</v>
@@ -3509,152 +3540,140 @@
         <v>60</v>
       </c>
       <c r="H58" t="s">
-        <v>177</v>
+        <v>257</v>
       </c>
       <c r="I58" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="K58" t="s">
-        <v>178</v>
+        <v>274</v>
       </c>
       <c r="M58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>251</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E59" t="s">
-        <v>98</v>
+        <v>255</v>
       </c>
       <c r="F59" t="s">
         <v>60</v>
       </c>
       <c r="H59" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="I59" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="K59" t="s">
-        <v>101</v>
+        <v>275</v>
       </c>
       <c r="M59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D60" t="s">
         <v>148</v>
       </c>
       <c r="E60" t="s">
-        <v>98</v>
+        <v>255</v>
       </c>
       <c r="F60" t="s">
         <v>60</v>
       </c>
       <c r="H60" t="s">
-        <v>179</v>
-      </c>
-      <c r="I60" t="s">
-        <v>180</v>
-      </c>
-      <c r="J60" t="s">
+        <v>258</v>
+      </c>
+      <c r="K60" t="s">
+        <v>276</v>
+      </c>
+      <c r="M60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="C61" t="s">
         <v>26</v>
-      </c>
-      <c r="K60" t="s">
-        <v>181</v>
-      </c>
-      <c r="M60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="C61" t="s">
-        <v>29</v>
       </c>
       <c r="D61" t="s">
         <v>148</v>
       </c>
       <c r="E61" t="s">
-        <v>98</v>
+        <v>255</v>
       </c>
       <c r="F61" t="s">
         <v>60</v>
       </c>
       <c r="H61" t="s">
-        <v>182</v>
+        <v>259</v>
       </c>
       <c r="I61" t="s">
-        <v>183</v>
-      </c>
-      <c r="J61" t="s">
-        <v>26</v>
+        <v>272</v>
       </c>
       <c r="K61" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="M61" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
         <v>148</v>
       </c>
       <c r="E62" t="s">
-        <v>98</v>
+        <v>255</v>
       </c>
       <c r="F62" t="s">
         <v>60</v>
       </c>
       <c r="H62" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I62" t="s">
-        <v>186</v>
-      </c>
-      <c r="J62" t="s">
-        <v>26</v>
+        <v>254</v>
       </c>
       <c r="K62" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="M62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D63" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E63" t="s">
         <v>98</v>
@@ -3663,27 +3682,24 @@
         <v>60</v>
       </c>
       <c r="H63" t="s">
-        <v>188</v>
+        <v>99</v>
       </c>
       <c r="I63" t="s">
-        <v>189</v>
-      </c>
-      <c r="J63" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="K63" t="s">
-        <v>190</v>
+        <v>101</v>
       </c>
       <c r="M63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>265</v>
+        <v>28</v>
       </c>
       <c r="D64" t="s">
         <v>148</v>
@@ -3695,27 +3711,27 @@
         <v>60</v>
       </c>
       <c r="H64" t="s">
-        <v>268</v>
+        <v>179</v>
       </c>
       <c r="I64" t="s">
-        <v>269</v>
+        <v>180</v>
       </c>
       <c r="J64" t="s">
         <v>26</v>
       </c>
       <c r="K64" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="M64" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>266</v>
+        <v>29</v>
       </c>
       <c r="D65" t="s">
         <v>148</v>
@@ -3727,27 +3743,27 @@
         <v>60</v>
       </c>
       <c r="H65" t="s">
-        <v>267</v>
+        <v>182</v>
       </c>
       <c r="I65" t="s">
-        <v>270</v>
+        <v>183</v>
       </c>
       <c r="J65" t="s">
         <v>26</v>
       </c>
       <c r="K65" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="M65" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D66" t="s">
         <v>148</v>
@@ -3759,27 +3775,27 @@
         <v>60</v>
       </c>
       <c r="H66" t="s">
-        <v>260</v>
+        <v>185</v>
       </c>
       <c r="I66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J66" t="s">
         <v>26</v>
       </c>
       <c r="K66" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M66" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>261</v>
+        <v>31</v>
       </c>
       <c r="D67" t="s">
         <v>148</v>
@@ -3791,27 +3807,27 @@
         <v>60</v>
       </c>
       <c r="H67" t="s">
-        <v>262</v>
+        <v>188</v>
       </c>
       <c r="I67" t="s">
-        <v>263</v>
+        <v>189</v>
       </c>
       <c r="J67" t="s">
         <v>26</v>
       </c>
       <c r="K67" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M67" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>33</v>
+        <v>265</v>
       </c>
       <c r="D68" t="s">
         <v>148</v>
@@ -3823,155 +3839,158 @@
         <v>60</v>
       </c>
       <c r="H68" t="s">
-        <v>194</v>
+        <v>268</v>
       </c>
       <c r="I68" t="s">
-        <v>195</v>
+        <v>269</v>
       </c>
       <c r="J68" t="s">
         <v>26</v>
       </c>
       <c r="K68" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M68" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>266</v>
       </c>
       <c r="D69" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E69" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F69" t="s">
         <v>60</v>
       </c>
       <c r="H69" t="s">
-        <v>89</v>
+        <v>267</v>
       </c>
       <c r="I69" t="s">
-        <v>311</v>
+        <v>270</v>
       </c>
       <c r="J69" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="K69" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="M69" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="D70" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E70" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F70" t="s">
         <v>60</v>
       </c>
       <c r="H70" t="s">
-        <v>92</v>
+        <v>260</v>
       </c>
       <c r="I70" t="s">
-        <v>312</v>
+        <v>191</v>
       </c>
       <c r="J70" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="K70" t="s">
-        <v>93</v>
+        <v>192</v>
       </c>
       <c r="M70" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="D71" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E71" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F71" t="s">
         <v>60</v>
       </c>
       <c r="H71" t="s">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="I71" t="s">
-        <v>104</v>
+        <v>263</v>
       </c>
       <c r="J71" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="K71" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
       <c r="M71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D72" t="s">
         <v>148</v>
       </c>
       <c r="E72" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F72" t="s">
         <v>60</v>
       </c>
       <c r="H72" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="I72" t="s">
-        <v>163</v>
+        <v>195</v>
+      </c>
+      <c r="J72" t="s">
+        <v>26</v>
       </c>
       <c r="K72" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="M72" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D73" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E73" t="s">
         <v>88</v>
@@ -3980,295 +3999,420 @@
         <v>60</v>
       </c>
       <c r="H73" t="s">
-        <v>202</v>
+        <v>89</v>
       </c>
       <c r="I73" t="s">
-        <v>203</v>
+        <v>311</v>
       </c>
       <c r="J73" t="s">
         <v>78</v>
       </c>
       <c r="K73" t="s">
-        <v>204</v>
+        <v>90</v>
       </c>
       <c r="M73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="D74" t="s">
         <v>43</v>
       </c>
       <c r="E74" t="s">
-        <v>242</v>
+        <v>88</v>
       </c>
       <c r="F74" t="s">
         <v>60</v>
       </c>
       <c r="H74" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="I74" t="s">
-        <v>304</v>
+        <v>312</v>
+      </c>
+      <c r="J74" t="s">
+        <v>66</v>
       </c>
       <c r="K74" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="M74" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="D75" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="E75" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="F75" t="s">
         <v>60</v>
       </c>
       <c r="H75" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="I75" t="s">
-        <v>19</v>
+        <v>104</v>
+      </c>
+      <c r="J75" t="s">
+        <v>15</v>
       </c>
       <c r="K75" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="M75" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="D76" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F76" t="s">
         <v>60</v>
       </c>
       <c r="H76" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="I76" t="s">
-        <v>309</v>
+        <v>163</v>
       </c>
       <c r="K76" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="M76" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D77" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E77" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F77" t="s">
         <v>60</v>
       </c>
       <c r="H77" t="s">
-        <v>76</v>
+        <v>202</v>
       </c>
       <c r="I77" t="s">
-        <v>77</v>
+        <v>203</v>
       </c>
       <c r="J77" t="s">
         <v>78</v>
       </c>
       <c r="K77" t="s">
-        <v>79</v>
+        <v>204</v>
       </c>
       <c r="M77" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D78" t="s">
         <v>43</v>
       </c>
       <c r="E78" t="s">
-        <v>72</v>
+        <v>242</v>
       </c>
       <c r="F78" t="s">
         <v>60</v>
       </c>
       <c r="H78" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="I78" t="s">
-        <v>108</v>
+        <v>304</v>
       </c>
       <c r="K78" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="M78" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="E79" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="F79" t="s">
         <v>60</v>
       </c>
       <c r="H79" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="I79" t="s">
-        <v>313</v>
+        <v>19</v>
       </c>
       <c r="K79" t="s">
-        <v>97</v>
+        <v>166</v>
       </c>
       <c r="M79" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="D80" t="s">
         <v>43</v>
       </c>
       <c r="E80" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F80" t="s">
         <v>60</v>
       </c>
       <c r="H80" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="I80" t="s">
-        <v>112</v>
-      </c>
-      <c r="J80" t="s">
-        <v>78</v>
+        <v>309</v>
       </c>
       <c r="K80" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="M80" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="D81" t="s">
         <v>43</v>
       </c>
       <c r="E81" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F81" t="s">
         <v>60</v>
       </c>
       <c r="H81" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="I81" t="s">
-        <v>116</v>
+        <v>77</v>
+      </c>
+      <c r="J81" t="s">
+        <v>78</v>
       </c>
       <c r="K81" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="M81" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" t="s">
+        <v>72</v>
+      </c>
+      <c r="F82" t="s">
+        <v>60</v>
+      </c>
+      <c r="H82" t="s">
+        <v>107</v>
+      </c>
+      <c r="I82" t="s">
+        <v>108</v>
+      </c>
+      <c r="K82" t="s">
+        <v>109</v>
+      </c>
+      <c r="M82" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" t="s">
+        <v>60</v>
+      </c>
+      <c r="H83" t="s">
+        <v>96</v>
+      </c>
+      <c r="I83" t="s">
+        <v>313</v>
+      </c>
+      <c r="K83" t="s">
+        <v>97</v>
+      </c>
+      <c r="M83" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>110</v>
+      </c>
+      <c r="D84" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" t="s">
+        <v>95</v>
+      </c>
+      <c r="F84" t="s">
+        <v>60</v>
+      </c>
+      <c r="H84" t="s">
+        <v>111</v>
+      </c>
+      <c r="I84" t="s">
+        <v>112</v>
+      </c>
+      <c r="J84" t="s">
+        <v>78</v>
+      </c>
+      <c r="K84" t="s">
+        <v>113</v>
+      </c>
+      <c r="M84" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" t="s">
+        <v>95</v>
+      </c>
+      <c r="F85" t="s">
+        <v>60</v>
+      </c>
+      <c r="H85" t="s">
+        <v>115</v>
+      </c>
+      <c r="I85" t="s">
+        <v>116</v>
+      </c>
+      <c r="K85" t="s">
+        <v>117</v>
+      </c>
+      <c r="M85" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
         <v>207</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C86" t="s">
         <v>38</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D86" t="s">
         <v>148</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E86" t="s">
         <v>95</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F86" t="s">
         <v>51</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H86" t="s">
         <v>208</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I86" t="s">
         <v>209</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K86" t="s">
         <v>210</v>
       </c>
-      <c r="M82" t="s">
+      <c r="M86" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M86" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M86">
-      <sortCondition ref="A1:A86"/>
+  <autoFilter ref="A1:M90" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M90">
+      <sortCondition ref="A1:A90"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4283,14 +4427,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4299,7 +4443,7 @@
         <v>HA_GEM_G;HA_HWA_G</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4308,7 +4452,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>247</v>
       </c>
@@ -4317,7 +4461,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>248</v>
       </c>
@@ -4326,7 +4470,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -4335,7 +4479,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>251</v>
       </c>
@@ -4344,7 +4488,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4353,7 +4497,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G;HA_OBK_G</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4362,7 +4506,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G;HA_OBK_G;HA_BEM_G</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4371,7 +4515,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G;HA_OBK_G;HA_BEM_G;HA_VER_G</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>271</v>
       </c>

</xml_diff>

<commit_message>
update model 1 and vbo bag
</commit_message>
<xml_diff>
--- a/inp_fields.xlsx
+++ b/inp_fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b_kro\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\GeoDynGemGWSW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\02_Werkplaatsen\07_IAN\bk\projecten\GeoDynGem\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2055030E-6A80-4B0E-9AD5-E7D48EDC9D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88408A1E-5F1F-4011-BC06-77B0952E8226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inp_fields" sheetId="1" r:id="rId1"/>
@@ -704,12 +704,6 @@
     <t>[ExAFW_4050_sum]</t>
   </si>
   <si>
-    <t>[par_result_count]</t>
-  </si>
-  <si>
-    <t>[zak_result_count]</t>
-  </si>
-  <si>
     <t>[par_result_sum]+[zak_result_sum]</t>
   </si>
   <si>
@@ -966,6 +960,12 @@
   </si>
   <si>
     <t xml:space="preserve"> if([BergendVermogen]/[POC_B_M3_T]&lt; 10,  [BergendVermogen]/[POC_B_M3_T], 10 + ([BergendVermogen] - 10*[POC_B_M3_T])/ [Pompcapaciteit_m3_u])</t>
+  </si>
+  <si>
+    <t>[vbo_fid_count]</t>
+  </si>
+  <si>
+    <t>[GRONDSLAG_sum]</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1492,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
@@ -1795,20 +1791,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="5" max="5" width="10.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.69921875" customWidth="1"/>
+    <col min="9" max="9" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1875,7 +1871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1901,12 +1897,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -1918,16 +1914,16 @@
         <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1947,7 +1943,7 @@
         <v>1000</v>
       </c>
       <c r="H5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K5" t="s">
         <v>139</v>
@@ -1956,12 +1952,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -1976,7 +1972,7 @@
         <v>1000</v>
       </c>
       <c r="H6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K6" t="s">
         <v>139</v>
@@ -1985,7 +1981,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2005,7 +2001,7 @@
         <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K7" t="s">
         <v>142</v>
@@ -2014,12 +2010,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
@@ -2043,12 +2039,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -2063,7 +2059,7 @@
         <v>1000</v>
       </c>
       <c r="H9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K9" t="s">
         <v>139</v>
@@ -2072,12 +2068,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
@@ -2101,7 +2097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2121,7 +2117,7 @@
         <v>149</v>
       </c>
       <c r="I11" t="s">
-        <v>222</v>
+        <v>308</v>
       </c>
       <c r="K11" t="s">
         <v>150</v>
@@ -2130,7 +2126,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2150,7 +2146,7 @@
         <v>153</v>
       </c>
       <c r="I12" t="s">
-        <v>223</v>
+        <v>309</v>
       </c>
       <c r="K12" t="s">
         <v>154</v>
@@ -2159,7 +2155,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2188,7 +2184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2217,7 +2213,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2246,7 +2242,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2275,7 +2271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2304,7 +2300,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2333,7 +2329,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2353,7 +2349,7 @@
         <v>144</v>
       </c>
       <c r="I19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K19" t="s">
         <v>145</v>
@@ -2362,7 +2358,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2394,7 +2390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2414,7 +2410,7 @@
         <v>59</v>
       </c>
       <c r="H21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K21" t="s">
         <v>60</v>
@@ -2423,7 +2419,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2452,7 +2448,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2472,7 +2468,7 @@
         <v>59</v>
       </c>
       <c r="H23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K23" t="s">
         <v>85</v>
@@ -2481,7 +2477,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2510,7 +2506,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2539,7 +2535,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2571,245 +2567,245 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C27" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D27" t="s">
         <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
       </c>
       <c r="H27" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I27" t="s">
         <v>83</v>
       </c>
       <c r="K27" t="s">
+        <v>280</v>
+      </c>
+      <c r="M27" t="s">
         <v>282</v>
       </c>
-      <c r="M27" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D28" t="s">
         <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F28" t="s">
         <v>59</v>
       </c>
       <c r="H28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I28" t="s">
         <v>57</v>
       </c>
       <c r="K28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M28" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D29" t="s">
         <v>42</v>
       </c>
       <c r="E29" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F29" t="s">
         <v>59</v>
       </c>
       <c r="H29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I29" t="s">
         <v>79</v>
       </c>
       <c r="K29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M29" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D30" t="s">
         <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F30" t="s">
         <v>50</v>
       </c>
       <c r="H30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I30" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M30" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D31" t="s">
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F31" t="s">
         <v>50</v>
       </c>
       <c r="H31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I31" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M31" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
       </c>
       <c r="H32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M32" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F33" t="s">
         <v>50</v>
       </c>
       <c r="H33" t="s">
+        <v>290</v>
+      </c>
+      <c r="I33" t="s">
         <v>292</v>
       </c>
-      <c r="I33" t="s">
-        <v>294</v>
-      </c>
       <c r="K33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M33" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F34" t="s">
         <v>50</v>
       </c>
       <c r="H34" t="s">
+        <v>291</v>
+      </c>
+      <c r="I34" t="s">
         <v>293</v>
       </c>
-      <c r="I34" t="s">
-        <v>295</v>
-      </c>
       <c r="K34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M34" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2838,7 +2834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2867,7 +2863,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2896,12 +2892,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D38" t="s">
         <v>143</v>
@@ -2925,12 +2921,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D39" t="s">
         <v>143</v>
@@ -2954,12 +2950,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D40" t="s">
         <v>143</v>
@@ -2983,12 +2979,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D41" t="s">
         <v>143</v>
@@ -3012,7 +3008,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3041,7 +3037,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3070,7 +3066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3099,12 +3095,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
@@ -3116,10 +3112,10 @@
         <v>59</v>
       </c>
       <c r="H45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I45" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K45" t="s">
         <v>135</v>
@@ -3128,12 +3124,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D46" t="s">
         <v>42</v>
@@ -3145,10 +3141,10 @@
         <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K46" t="s">
         <v>136</v>
@@ -3157,12 +3153,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
@@ -3174,10 +3170,10 @@
         <v>59</v>
       </c>
       <c r="H47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I47" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K47" t="s">
         <v>135</v>
@@ -3186,12 +3182,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D48" t="s">
         <v>42</v>
@@ -3203,10 +3199,10 @@
         <v>59</v>
       </c>
       <c r="H48" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="K48" t="s">
         <v>136</v>
@@ -3215,7 +3211,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3244,7 +3240,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3273,7 +3269,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3287,7 +3283,7 @@
         <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F51" t="s">
         <v>59</v>
@@ -3296,7 +3292,7 @@
         <v>164</v>
       </c>
       <c r="I51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K51" t="s">
         <v>165</v>
@@ -3305,7 +3301,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3316,7 +3312,7 @@
         <v>143</v>
       </c>
       <c r="E52" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F52" t="s">
         <v>59</v>
@@ -3325,7 +3321,7 @@
         <v>169</v>
       </c>
       <c r="I52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K52" t="s">
         <v>170</v>
@@ -3334,7 +3330,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3348,7 +3344,7 @@
         <v>143</v>
       </c>
       <c r="E53" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F53" t="s">
         <v>59</v>
@@ -3357,7 +3353,7 @@
         <v>167</v>
       </c>
       <c r="I53" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K53" t="s">
         <v>168</v>
@@ -3366,7 +3362,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3374,22 +3370,22 @@
         <v>163</v>
       </c>
       <c r="C54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D54" t="s">
         <v>143</v>
       </c>
       <c r="E54" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F54" t="s">
         <v>59</v>
       </c>
       <c r="H54" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I54" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K54" t="s">
         <v>165</v>
@@ -3398,36 +3394,36 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D55" t="s">
         <v>143</v>
       </c>
       <c r="E55" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
       </c>
       <c r="H55" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I55" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K55" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3438,54 +3434,54 @@
         <v>143</v>
       </c>
       <c r="E56" t="s">
+        <v>245</v>
+      </c>
+      <c r="F56" t="s">
+        <v>59</v>
+      </c>
+      <c r="H56" t="s">
         <v>247</v>
       </c>
-      <c r="F56" t="s">
-        <v>59</v>
-      </c>
-      <c r="H56" t="s">
-        <v>249</v>
-      </c>
       <c r="I56" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D57" t="s">
         <v>143</v>
       </c>
       <c r="E57" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F57" t="s">
         <v>59</v>
       </c>
       <c r="H57" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I57" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K57" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>58</v>
       </c>
@@ -3496,16 +3492,16 @@
         <v>143</v>
       </c>
       <c r="E58" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F58" t="s">
         <v>59</v>
       </c>
       <c r="H58" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I58" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K58" t="s">
         <v>171</v>
@@ -3514,7 +3510,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>59</v>
       </c>
@@ -3525,7 +3521,7 @@
         <v>143</v>
       </c>
       <c r="E59" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F59" t="s">
         <v>59</v>
@@ -3534,7 +3530,7 @@
         <v>172</v>
       </c>
       <c r="I59" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K59" t="s">
         <v>173</v>
@@ -3543,7 +3539,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>60</v>
       </c>
@@ -3572,7 +3568,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>61</v>
       </c>
@@ -3604,7 +3600,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>62</v>
       </c>
@@ -3636,7 +3632,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>63</v>
       </c>
@@ -3668,7 +3664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>64</v>
       </c>
@@ -3700,12 +3696,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>65</v>
       </c>
       <c r="C65" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D65" t="s">
         <v>143</v>
@@ -3717,10 +3713,10 @@
         <v>59</v>
       </c>
       <c r="H65" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I65" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J65" t="s">
         <v>26</v>
@@ -3732,12 +3728,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D66" t="s">
         <v>143</v>
@@ -3749,10 +3745,10 @@
         <v>59</v>
       </c>
       <c r="H66" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I66" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J66" t="s">
         <v>26</v>
@@ -3764,7 +3760,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>67</v>
       </c>
@@ -3781,7 +3777,7 @@
         <v>59</v>
       </c>
       <c r="H67" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I67" t="s">
         <v>186</v>
@@ -3796,12 +3792,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>68</v>
       </c>
       <c r="C68" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D68" t="s">
         <v>143</v>
@@ -3813,10 +3809,10 @@
         <v>59</v>
       </c>
       <c r="H68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J68" t="s">
         <v>26</v>
@@ -3828,7 +3824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>70</v>
       </c>
@@ -3848,7 +3844,7 @@
         <v>88</v>
       </c>
       <c r="I69" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J69" t="s">
         <v>77</v>
@@ -3860,7 +3856,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>71</v>
       </c>
@@ -3880,7 +3876,7 @@
         <v>91</v>
       </c>
       <c r="I70" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J70" t="s">
         <v>65</v>
@@ -3892,7 +3888,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>72</v>
       </c>
@@ -3924,7 +3920,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>73</v>
       </c>
@@ -3953,7 +3949,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>74</v>
       </c>
@@ -3985,7 +3981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>75</v>
       </c>
@@ -3996,7 +3992,7 @@
         <v>42</v>
       </c>
       <c r="E74" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F74" t="s">
         <v>59</v>
@@ -4005,7 +4001,7 @@
         <v>63</v>
       </c>
       <c r="I74" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K74" t="s">
         <v>64</v>
@@ -4014,7 +4010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>76</v>
       </c>
@@ -4043,7 +4039,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>77</v>
       </c>
@@ -4063,7 +4059,7 @@
         <v>72</v>
       </c>
       <c r="I76" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K76" t="s">
         <v>73</v>
@@ -4072,7 +4068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>78</v>
       </c>
@@ -4104,7 +4100,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>79</v>
       </c>
@@ -4133,7 +4129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>80</v>
       </c>
@@ -4153,7 +4149,7 @@
         <v>95</v>
       </c>
       <c r="I79" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="K79" t="s">
         <v>96</v>
@@ -4162,7 +4158,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>81</v>
       </c>
@@ -4194,7 +4190,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>82</v>
       </c>
@@ -4223,7 +4219,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>83</v>
       </c>
@@ -4273,14 +4269,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4289,7 +4285,7 @@
         <v>HA_GEM_G;HA_HWA_G</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4298,25 +4294,25 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B10" si="0">B3&amp;";"&amp;A4</f>
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -4325,16 +4321,16 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4343,7 +4339,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G;HA_OBK_G</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4352,7 +4348,7 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G;HA_OBK_G;HA_BEM_G</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4361,9 +4357,9 @@
         <v>HA_GEM_G;HA_HWA_G;HA_VGS_G;HA_VWR_G;HA_INF_G;HA_OPW_G;HA_MVD_G;HA_OBK_G;HA_BEM_G;HA_VER_G</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>